<commit_message>
add shunt and generator
</commit_message>
<xml_diff>
--- a/Files/nodes_branches_3.xlsx
+++ b/Files/nodes_branches_3.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\pandapower\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\pandapower\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="8832"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="8835"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="2" r:id="rId1"/>
     <sheet name="branch" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>r</t>
   </si>
@@ -79,12 +79,21 @@
   </si>
   <si>
     <t>qmax</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>bsh</t>
+  </si>
+  <si>
+    <t>base</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -397,18 +406,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -445,8 +454,14 @@
       <c r="L1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -483,8 +498,14 @@
       <c r="L2">
         <v>9999</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -521,8 +542,11 @@
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -559,8 +583,11 @@
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -597,8 +624,11 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -635,8 +665,11 @@
       <c r="L6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -673,8 +706,11 @@
       <c r="L7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -709,6 +745,9 @@
         <v>0</v>
       </c>
       <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>0</v>
       </c>
     </row>
@@ -725,12 +764,12 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -753,7 +792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -776,7 +815,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -799,7 +838,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -822,7 +861,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -845,7 +884,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -868,7 +907,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -891,7 +930,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -914,7 +953,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>

</xml_diff>